<commit_message>
fix disparity error type issue uint8 -> int32
</commit_message>
<xml_diff>
--- a/warping_dataset/bike/testing.xlsx
+++ b/warping_dataset/bike/testing.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,20 +447,305 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>23.66698125826089</v>
       </c>
       <c r="C2" t="n">
-        <v>23.75720439392547</v>
+        <v>23.42013439223523</v>
       </c>
       <c r="D2" t="n">
         <v>0.5628382013489843</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5805919008384031</v>
+        <v>0.5804712546134158</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>23.6652446485445</v>
+      </c>
+      <c r="C3" t="n">
+        <v>24.05579222437616</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.5628585081383963</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.613742543171837</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>23.66542198747178</v>
+      </c>
+      <c r="C4" t="n">
+        <v>25.43849144375257</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.5615749372769705</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.6842200997350938</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>23.6659291784576</v>
+      </c>
+      <c r="C5" t="n">
+        <v>29.09421076393417</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.5617109537252648</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.8316405635363789</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>23.61109032665684</v>
+      </c>
+      <c r="C6" t="n">
+        <v>22.7552839708626</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.5630425821079695</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.5316978520688432</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>23.56698259185531</v>
+      </c>
+      <c r="C7" t="n">
+        <v>23.31498834013616</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.560701678971915</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.565062299647228</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>23.61746968066501</v>
+      </c>
+      <c r="C8" t="n">
+        <v>24.7460004079343</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.5623654053350033</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.6464005945857576</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>23.67097614796583</v>
+      </c>
+      <c r="C9" t="n">
+        <v>28.35847660851668</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.5623341805466151</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.8031275800649054</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>23.58185794894158</v>
+      </c>
+      <c r="C10" t="n">
+        <v>28.29419717316968</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.5592424193153306</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.8042189327551276</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>23.53296335514261</v>
+      </c>
+      <c r="C11" t="n">
+        <v>24.70011184212721</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.5607680889382359</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.6485018772956437</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>23.53707245832457</v>
+      </c>
+      <c r="C12" t="n">
+        <v>23.336184782947</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.5618308869854264</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.5707600925522629</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>23.62904466930573</v>
+      </c>
+      <c r="C13" t="n">
+        <v>22.87548817301593</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.563244054210409</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.5375440827307707</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>23.60078928168511</v>
+      </c>
+      <c r="C14" t="n">
+        <v>29.09656297293069</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.5629599752400475</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.8334006987874809</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>23.59847117915199</v>
+      </c>
+      <c r="C15" t="n">
+        <v>25.4901777388197</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.5619946590095188</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.6862067042922995</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>23.59772295605822</v>
+      </c>
+      <c r="C16" t="n">
+        <v>24.04720191284321</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.5586627486975914</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.6104305880609839</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>23.59866594249343</v>
+      </c>
+      <c r="C17" t="n">
+        <v>23.37781593296855</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.5600088516890556</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.5763392919183502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add occlusion + unwarped matrix
</commit_message>
<xml_diff>
--- a/warping_dataset/bike/testing.xlsx
+++ b/warping_dataset/bike/testing.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,13 +454,13 @@
         <v>23.66698125826089</v>
       </c>
       <c r="C2" t="n">
-        <v>23.42013439223523</v>
+        <v>23.26790258615237</v>
       </c>
       <c r="D2" t="n">
         <v>0.5628382013489843</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5804712546134158</v>
+        <v>0.5691875071735751</v>
       </c>
     </row>
     <row r="3">
@@ -473,13 +473,13 @@
         <v>23.6652446485445</v>
       </c>
       <c r="C3" t="n">
-        <v>24.05579222437616</v>
+        <v>23.95886060057096</v>
       </c>
       <c r="D3" t="n">
         <v>0.5628585081383963</v>
       </c>
       <c r="E3" t="n">
-        <v>0.613742543171837</v>
+        <v>0.6050178600059178</v>
       </c>
     </row>
     <row r="4">
@@ -492,13 +492,13 @@
         <v>23.66542198747178</v>
       </c>
       <c r="C4" t="n">
-        <v>25.43849144375257</v>
+        <v>25.33142633381867</v>
       </c>
       <c r="D4" t="n">
         <v>0.5615749372769705</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6842200997350938</v>
+        <v>0.677828129208542</v>
       </c>
     </row>
     <row r="5">
@@ -511,241 +511,13 @@
         <v>23.6659291784576</v>
       </c>
       <c r="C5" t="n">
-        <v>29.09421076393417</v>
+        <v>28.71055627543781</v>
       </c>
       <c r="D5" t="n">
         <v>0.5617109537252648</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8316405635363789</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>23.61109032665684</v>
-      </c>
-      <c r="C6" t="n">
-        <v>22.7552839708626</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.5630425821079695</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.5316978520688432</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>23.56698259185531</v>
-      </c>
-      <c r="C7" t="n">
-        <v>23.31498834013616</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.560701678971915</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.565062299647228</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>23.61746968066501</v>
-      </c>
-      <c r="C8" t="n">
-        <v>24.7460004079343</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.5623654053350033</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.6464005945857576</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>23.67097614796583</v>
-      </c>
-      <c r="C9" t="n">
-        <v>28.35847660851668</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.5623341805466151</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.8031275800649054</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>23.58185794894158</v>
-      </c>
-      <c r="C10" t="n">
-        <v>28.29419717316968</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.5592424193153306</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.8042189327551276</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>23.53296335514261</v>
-      </c>
-      <c r="C11" t="n">
-        <v>24.70011184212721</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.5607680889382359</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.6485018772956437</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>23.53707245832457</v>
-      </c>
-      <c r="C12" t="n">
-        <v>23.336184782947</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.5618308869854264</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.5707600925522629</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>23.62904466930573</v>
-      </c>
-      <c r="C13" t="n">
-        <v>22.87548817301593</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.563244054210409</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.5375440827307707</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>23.60078928168511</v>
-      </c>
-      <c r="C14" t="n">
-        <v>29.09656297293069</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.5629599752400475</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.8334006987874809</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>23.59847117915199</v>
-      </c>
-      <c r="C15" t="n">
-        <v>25.4901777388197</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0.5619946590095188</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.6862067042922995</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>23.59772295605822</v>
-      </c>
-      <c r="C16" t="n">
-        <v>24.04720191284321</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0.5586627486975914</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.6104305880609839</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>23.59866594249343</v>
-      </c>
-      <c r="C17" t="n">
-        <v>23.37781593296855</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0.5600088516890556</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.5763392919183502</v>
+        <v>0.823414760904444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add fusion occlusion map code
</commit_message>
<xml_diff>
--- a/warping_dataset/bike/testing.xlsx
+++ b/warping_dataset/bike/testing.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,13 +454,13 @@
         <v>23.66698125826089</v>
       </c>
       <c r="C2" t="n">
-        <v>23.26790258615237</v>
+        <v>23.42013439223523</v>
       </c>
       <c r="D2" t="n">
         <v>0.5628382013489843</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5691875071735751</v>
+        <v>0.5804712546134158</v>
       </c>
     </row>
     <row r="3">
@@ -473,13 +473,13 @@
         <v>23.6652446485445</v>
       </c>
       <c r="C3" t="n">
-        <v>23.95886060057096</v>
+        <v>24.05579222437616</v>
       </c>
       <c r="D3" t="n">
         <v>0.5628585081383963</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6050178600059178</v>
+        <v>0.613742543171837</v>
       </c>
     </row>
     <row r="4">
@@ -492,13 +492,13 @@
         <v>23.66542198747178</v>
       </c>
       <c r="C4" t="n">
-        <v>25.33142633381867</v>
+        <v>25.43849144375257</v>
       </c>
       <c r="D4" t="n">
         <v>0.5615749372769705</v>
       </c>
       <c r="E4" t="n">
-        <v>0.677828129208542</v>
+        <v>0.6842200997350938</v>
       </c>
     </row>
     <row r="5">
@@ -511,13 +511,248 @@
         <v>23.6659291784576</v>
       </c>
       <c r="C5" t="n">
-        <v>28.71055627543781</v>
+        <v>29.09421076393417</v>
       </c>
       <c r="D5" t="n">
         <v>0.5617109537252648</v>
       </c>
       <c r="E5" t="n">
-        <v>0.823414760904444</v>
+        <v>0.8316405635363789</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>23.61109032665684</v>
+      </c>
+      <c r="C6" t="n">
+        <v>22.7552839708626</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.5630425821079695</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.5316978520688432</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>23.56698259185531</v>
+      </c>
+      <c r="C7" t="n">
+        <v>23.31498834013616</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.560701678971915</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.565062299647228</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>23.61746968066501</v>
+      </c>
+      <c r="C8" t="n">
+        <v>24.7460004079343</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.5623654053350033</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.6464005945857576</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>23.67097614796583</v>
+      </c>
+      <c r="C9" t="n">
+        <v>28.35847660851668</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.5623341805466151</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.8031275800649054</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>23.58185794894158</v>
+      </c>
+      <c r="C10" t="n">
+        <v>28.29419717316968</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.5592424193153306</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.8042189327551276</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>23.53296335514261</v>
+      </c>
+      <c r="C11" t="n">
+        <v>24.70011184212721</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.5607680889382359</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.6485018772956437</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>23.53707245832457</v>
+      </c>
+      <c r="C12" t="n">
+        <v>23.336184782947</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.5618308869854264</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.5707600925522629</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>23.62904466930573</v>
+      </c>
+      <c r="C13" t="n">
+        <v>22.87548817301593</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.563244054210409</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.5375440827307707</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>23.60078928168511</v>
+      </c>
+      <c r="C14" t="n">
+        <v>29.09656297293069</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.5629599752400475</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.8334006987874809</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>23.59847117915199</v>
+      </c>
+      <c r="C15" t="n">
+        <v>25.4901777388197</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.5619946590095188</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.6862067042922995</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>23.59772295605822</v>
+      </c>
+      <c r="C16" t="n">
+        <v>24.04720191284321</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.5586627486975914</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.6104305880609839</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>23.59866594249343</v>
+      </c>
+      <c r="C17" t="n">
+        <v>23.37781593296855</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.5600088516890556</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.5763392919183502</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>730.1483306884766</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>